<commit_message>
Needed to reverse values for ltu to prevent initialization error
</commit_message>
<xml_diff>
--- a/data/databook-simple-cascade-autocalibration.xlsx
+++ b/data/databook-simple-cascade-autocalibration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="-23540" windowWidth="25600" windowHeight="22500" activeTab="7"/>
+    <workbookView xWindow="260" yWindow="-23540" windowWidth="25600" windowHeight="22500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -1234,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1456,7 +1456,7 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="O7">
         <v>62500</v>
@@ -1677,7 +1677,7 @@
         <v>14</v>
       </c>
       <c r="E15">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="J15">
         <v>2200</v>
@@ -2263,7 +2263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>

</xml_diff>